<commit_message>
Minor changes and additions
- Removed unused imports
- Implemented dropdown list for semester selection in Course and Student Registration forms
- Added Excel file with 100 student registrations
- Changed some semester values in files-for-importing dir
</commit_message>
<xml_diff>
--- a/src/main/resources/files-for-importing/myy301_students.xlsx
+++ b/src/main/resources/files-for-importing/myy301_students.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Panos\CSE UOI\Personal_Projects\Course-Manager-Web-App\src\main\resources\csvFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Panos\CSE UOI\Personal_Projects\Course-Manager-Web-App\src\main\resources\files-for-importing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49754FC8-3F9D-47C6-A8A9-1E0830CB0E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6D493B-1B0B-4979-98E6-ACF67C936F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0505F9EA-C4AD-40FA-B926-7DBA97050A50}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0505F9EA-C4AD-40FA-B926-7DBA97050A50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="myy301_students" localSheetId="0">Sheet1!$A$1:$I$8</definedName>
+    <definedName name="myy301_students_1" localSheetId="0">Sheet1!$A$1:$I$8</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,8 +37,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{8926F491-B287-4399-A379-0C43B6331977}" name="myy301_students" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="737" sourceFile="D:\Panos\CSE UOI\Personal_Projects\Course-Manager-Web-App\src\main\resources\csvFiles\myy301_students.csv" tab="0" comma="1">
+  <connection id="1" xr16:uid="{5D36F923-4058-487D-B0CE-782D49C03D8D}" name="myy301_students" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="737" sourceFile="D:\Panos\CSE UOI\Personal_Projects\Course-Manager-Web-App\src\main\resources\files-for-importing\myy301_students.csv" tab="0" comma="1">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -56,35 +56,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
-  <si>
-    <t>AM</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Year of Registration</t>
-  </si>
-  <si>
-    <t>Year of Studies</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Semester</t>
   </si>
   <si>
-    <t>Course Id</t>
-  </si>
-  <si>
-    <t>Project Grade</t>
-  </si>
-  <si>
-    <t>Exam Grade</t>
-  </si>
-  <si>
     <t>Name3</t>
   </si>
   <si>
@@ -112,22 +88,49 @@
     <t>LName6</t>
   </si>
   <si>
-    <t xml:space="preserve"> Name7</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LName1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name8</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LName2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name9</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LName3</t>
+    <t>StudentId</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>RegistrationYear</t>
+  </si>
+  <si>
+    <t>YearOfStudies</t>
+  </si>
+  <si>
+    <t>CourseId</t>
+  </si>
+  <si>
+    <t>ProjectGrade</t>
+  </si>
+  <si>
+    <t>ExamGrade</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>Fall</t>
+  </si>
+  <si>
+    <t>LName1</t>
+  </si>
+  <si>
+    <t>LName2</t>
+  </si>
+  <si>
+    <t>Name7</t>
+  </si>
+  <si>
+    <t>Name8</t>
+  </si>
+  <si>
+    <t>Name9</t>
   </si>
 </sst>
 </file>
@@ -184,7 +187,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="myy301_students" connectionId="1" xr16:uid="{FAAD545B-1461-4D25-A75E-CE69D0604955}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="myy301_students_1" connectionId="1" xr16:uid="{C8AA79E4-C663-4FCC-AD21-E8AD7410F4F2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -487,60 +490,60 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>3333</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>2017</v>
@@ -548,11 +551,11 @@
       <c r="E2">
         <v>3</v>
       </c>
-      <c r="F2">
-        <v>5</v>
+      <c r="F2" t="s">
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H2">
         <v>2.5</v>
@@ -561,15 +564,15 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4444</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>1995</v>
@@ -577,11 +580,11 @@
       <c r="E3">
         <v>5</v>
       </c>
-      <c r="F3">
-        <v>10</v>
+      <c r="F3" t="s">
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H3">
         <v>8.5</v>
@@ -590,15 +593,15 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>5555</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>2021</v>
@@ -606,11 +609,11 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>1</v>
+      <c r="F4" t="s">
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H4">
         <v>4</v>
@@ -619,15 +622,15 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>6666</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>2018</v>
@@ -635,11 +638,11 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>2</v>
+      <c r="F5" t="s">
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H5">
         <v>6.5</v>
@@ -648,15 +651,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>7777</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6">
         <v>2000</v>
@@ -664,11 +667,11 @@
       <c r="E6">
         <v>2</v>
       </c>
-      <c r="F6">
-        <v>4</v>
+      <c r="F6" t="s">
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H6">
         <v>5</v>
@@ -677,12 +680,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>8888</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
@@ -693,11 +696,11 @@
       <c r="E7">
         <v>4</v>
       </c>
-      <c r="F7">
-        <v>5</v>
+      <c r="F7" t="s">
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H7">
         <v>5</v>
@@ -706,15 +709,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>9999</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="D8">
         <v>2003</v>
@@ -722,11 +725,11 @@
       <c r="E8">
         <v>5</v>
       </c>
-      <c r="F8">
-        <v>7</v>
+      <c r="F8" t="s">
+        <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H8">
         <v>1</v>

</xml_diff>